<commit_message>
- Migrated keywords, test cases and datasets - Added input and output filles - Adjusted path file settings in IEE environment and importfile.robot - Updated instance of FFC1CMUpdateSourceMQ
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/API/API_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/API/API_Data_Set.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="4" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="4" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="READ_ME" sheetId="1" state="visible" r:id="rId1"/>
@@ -55104,7 +55104,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E33" sqref="E33"/>
+      <selection pane="topRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -56076,12 +56076,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>S5A_12102019150225BIE</t>
+          <t>BNS1_28072020211931IFJ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ESPS51010132</t>
+          <t>CUSTLEGAL43149</t>
         </is>
       </c>
       <c r="E5" s="41" t="n"/>
@@ -56098,22 +56098,22 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>F$DZ9FAZ</t>
+          <t>.9EGB5MK</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>LIQ-F$DZ9FAZ-F$DZ9F8C-2</t>
+          <t>LIQ-.9EGB5MK-.9EGB5KD-43</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2021-05-08 00:00:00.000</t>
+          <t>2023-02-03 00:00:00.000</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2016-12-20 00:00:00.000</t>
+          <t>2018-09-17 00:00:00.000</t>
         </is>
       </c>
       <c r="M5" s="78" t="n">

</xml_diff>

<commit_message>
- Migrated keywords and related datasets for API_CORRO_TCO3 - Added writing of deal,facility and loan alias to corro api dataset on Scenario 1 Deal
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/API/API_Data_Set.xlsx
+++ b/DataSet/Integration_DataSet/API/API_Data_Set.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\GDE-6487\DataSet\Integration_DataSet\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\GDE-TC03\DataSet\Integration_DataSet\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABE567-6F09-4DFB-9002-60FDE15DBC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED448FBA-D525-47A6-A4B5-1A67E0A6508F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13450" uniqueCount="4181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13450" uniqueCount="4183">
   <si>
     <t>Users API Guide</t>
   </si>
@@ -12604,6 +12604,12 @@
   </si>
   <si>
     <t>API_RESPONSE_PTY_CRE07CS</t>
+  </si>
+  <si>
+    <t>ATM BILAT AUD108.6M 29JUN15</t>
+  </si>
+  <si>
+    <t>FACILITY RENEW</t>
   </si>
 </sst>
 </file>
@@ -13208,28 +13214,11 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -13243,6 +13232,26 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -13254,9 +13263,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -13592,968 +13598,974 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="90"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="104"/>
     </row>
     <row r="2" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="92"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="92"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="89"/>
     </row>
     <row r="4" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="92"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="89"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="92"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="89"/>
     </row>
     <row r="6" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="92"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="89"/>
     </row>
     <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="92"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="89"/>
     </row>
     <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
-      <c r="O8" s="92"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="89"/>
     </row>
     <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="93"/>
-      <c r="N9" s="93"/>
-      <c r="O9" s="92"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="89"/>
     </row>
     <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="93"/>
-      <c r="N10" s="93"/>
-      <c r="O10" s="92"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="89"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="93"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="92"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="89"/>
     </row>
     <row r="12" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="93"/>
-      <c r="N12" s="93"/>
-      <c r="O12" s="92"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="89"/>
     </row>
     <row r="13" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
-      <c r="O13" s="92"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="89"/>
     </row>
     <row r="14" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="93"/>
-      <c r="N14" s="93"/>
-      <c r="O14" s="92"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="89"/>
     </row>
     <row r="15" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="92"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="92"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="89"/>
     </row>
     <row r="16" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="98" t="s">
+      <c r="A16" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="100"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="93"/>
     </row>
     <row r="17" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="101"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="93"/>
-      <c r="N17" s="93"/>
-      <c r="O17" s="102"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="95"/>
     </row>
     <row r="18" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="101"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93"/>
-      <c r="M18" s="93"/>
-      <c r="N18" s="93"/>
-      <c r="O18" s="102"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="95"/>
     </row>
     <row r="19" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="101"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="93"/>
-      <c r="N19" s="93"/>
-      <c r="O19" s="102"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="95"/>
     </row>
     <row r="20" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="101"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="102"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="95"/>
     </row>
     <row r="21" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="101"/>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="92"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="102"/>
+      <c r="A21" s="94"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="90"/>
+      <c r="O21" s="95"/>
     </row>
     <row r="22" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="101"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="93"/>
-      <c r="J22" s="93"/>
-      <c r="K22" s="93"/>
-      <c r="L22" s="93"/>
-      <c r="M22" s="93"/>
-      <c r="N22" s="93"/>
-      <c r="O22" s="102"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="95"/>
     </row>
     <row r="23" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="101"/>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="93"/>
-      <c r="J23" s="93"/>
-      <c r="K23" s="93"/>
-      <c r="L23" s="93"/>
-      <c r="M23" s="93"/>
-      <c r="N23" s="93"/>
-      <c r="O23" s="102"/>
+      <c r="A23" s="94"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
+      <c r="O23" s="95"/>
     </row>
     <row r="24" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="101"/>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="93"/>
-      <c r="K24" s="93"/>
-      <c r="L24" s="93"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="93"/>
-      <c r="O24" s="102"/>
+      <c r="A24" s="94"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="95"/>
     </row>
     <row r="25" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="101"/>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="93"/>
-      <c r="L25" s="93"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
-      <c r="O25" s="102"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="95"/>
     </row>
     <row r="26" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="101"/>
-      <c r="B26" s="92"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="93"/>
-      <c r="K26" s="93"/>
-      <c r="L26" s="93"/>
-      <c r="M26" s="93"/>
-      <c r="N26" s="93"/>
-      <c r="O26" s="102"/>
+      <c r="A26" s="94"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="95"/>
     </row>
     <row r="27" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="103"/>
-      <c r="B27" s="104"/>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104"/>
-      <c r="I27" s="104"/>
-      <c r="J27" s="104"/>
-      <c r="K27" s="104"/>
-      <c r="L27" s="104"/>
-      <c r="M27" s="104"/>
-      <c r="N27" s="104"/>
-      <c r="O27" s="105"/>
+      <c r="A27" s="96"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="98"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="97"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="89"/>
-      <c r="O28" s="90"/>
+      <c r="A28" s="105"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="103"/>
+      <c r="K28" s="103"/>
+      <c r="L28" s="103"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="103"/>
+      <c r="O28" s="104"/>
     </row>
     <row r="29" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="96" t="s">
+      <c r="A29" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="89"/>
-      <c r="N29" s="89"/>
-      <c r="O29" s="90"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="104"/>
     </row>
     <row r="30" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="93"/>
-      <c r="M30" s="93"/>
-      <c r="N30" s="93"/>
-      <c r="O30" s="92"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="89"/>
     </row>
     <row r="31" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94" t="s">
+      <c r="A31" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="L31" s="93"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="93"/>
-      <c r="O31" s="92"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="90"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="90"/>
+      <c r="N31" s="90"/>
+      <c r="O31" s="89"/>
     </row>
     <row r="32" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="93"/>
-      <c r="O32" s="92"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
+      <c r="O32" s="89"/>
     </row>
     <row r="33" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="91" t="s">
+      <c r="A33" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="92"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="92"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="90"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="89"/>
     </row>
     <row r="34" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="92"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="92"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="89"/>
     </row>
     <row r="35" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="94" t="s">
+      <c r="A35" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="92"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="93"/>
-      <c r="N35" s="93"/>
-      <c r="O35" s="92"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="89"/>
     </row>
     <row r="36" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="91" t="s">
+      <c r="A36" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="92"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
-      <c r="K36" s="93"/>
-      <c r="L36" s="93"/>
-      <c r="M36" s="93"/>
-      <c r="N36" s="93"/>
-      <c r="O36" s="92"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="90"/>
+      <c r="I36" s="90"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="89"/>
     </row>
     <row r="37" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="95" t="s">
+      <c r="A37" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="93"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
-      <c r="K37" s="93"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="93"/>
-      <c r="N37" s="93"/>
-      <c r="O37" s="92"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="90"/>
+      <c r="F37" s="90"/>
+      <c r="G37" s="90"/>
+      <c r="H37" s="90"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="90"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="89"/>
     </row>
     <row r="38" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="92"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="93"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="93"/>
-      <c r="I38" s="93"/>
-      <c r="J38" s="93"/>
-      <c r="K38" s="93"/>
-      <c r="L38" s="93"/>
-      <c r="M38" s="93"/>
-      <c r="N38" s="93"/>
-      <c r="O38" s="92"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="90"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="90"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="90"/>
+      <c r="N38" s="90"/>
+      <c r="O38" s="89"/>
     </row>
     <row r="39" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
-      <c r="O39" s="92"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="90"/>
+      <c r="N39" s="90"/>
+      <c r="O39" s="89"/>
     </row>
     <row r="40" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106"/>
-      <c r="B40" s="104"/>
-      <c r="C40" s="104"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="104"/>
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="104"/>
-      <c r="I40" s="104"/>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
-      <c r="N40" s="104"/>
-      <c r="O40" s="105"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="97"/>
+      <c r="H40" s="97"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="97"/>
+      <c r="K40" s="97"/>
+      <c r="L40" s="97"/>
+      <c r="M40" s="97"/>
+      <c r="N40" s="97"/>
+      <c r="O40" s="98"/>
     </row>
     <row r="41" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="98" t="s">
+      <c r="A41" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="99"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="99"/>
-      <c r="M41" s="99"/>
-      <c r="N41" s="99"/>
-      <c r="O41" s="100"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="92"/>
+      <c r="L41" s="92"/>
+      <c r="M41" s="92"/>
+      <c r="N41" s="92"/>
+      <c r="O41" s="93"/>
     </row>
     <row r="42" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="101"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="93"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="93"/>
-      <c r="L42" s="93"/>
-      <c r="M42" s="93"/>
-      <c r="N42" s="93"/>
-      <c r="O42" s="102"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
+      <c r="N42" s="90"/>
+      <c r="O42" s="95"/>
     </row>
     <row r="43" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="101"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="93"/>
-      <c r="N43" s="93"/>
-      <c r="O43" s="102"/>
+      <c r="A43" s="94"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="90"/>
+      <c r="H43" s="90"/>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="90"/>
+      <c r="N43" s="90"/>
+      <c r="O43" s="95"/>
     </row>
     <row r="44" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="101"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="93"/>
-      <c r="F44" s="93"/>
-      <c r="G44" s="93"/>
-      <c r="H44" s="93"/>
-      <c r="I44" s="93"/>
-      <c r="J44" s="93"/>
-      <c r="K44" s="93"/>
-      <c r="L44" s="93"/>
-      <c r="M44" s="93"/>
-      <c r="N44" s="93"/>
-      <c r="O44" s="102"/>
+      <c r="A44" s="94"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="90"/>
+      <c r="N44" s="90"/>
+      <c r="O44" s="95"/>
     </row>
     <row r="45" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="101"/>
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="93"/>
-      <c r="F45" s="93"/>
-      <c r="G45" s="93"/>
-      <c r="H45" s="93"/>
-      <c r="I45" s="93"/>
-      <c r="J45" s="93"/>
-      <c r="K45" s="93"/>
-      <c r="L45" s="93"/>
-      <c r="M45" s="93"/>
-      <c r="N45" s="93"/>
-      <c r="O45" s="102"/>
+      <c r="A45" s="94"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
+      <c r="M45" s="90"/>
+      <c r="N45" s="90"/>
+      <c r="O45" s="95"/>
     </row>
     <row r="46" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="101"/>
-      <c r="B46" s="92"/>
-      <c r="C46" s="92"/>
-      <c r="D46" s="92"/>
-      <c r="E46" s="93"/>
-      <c r="F46" s="93"/>
-      <c r="G46" s="93"/>
-      <c r="H46" s="93"/>
-      <c r="I46" s="93"/>
-      <c r="J46" s="93"/>
-      <c r="K46" s="93"/>
-      <c r="L46" s="93"/>
-      <c r="M46" s="93"/>
-      <c r="N46" s="93"/>
-      <c r="O46" s="102"/>
+      <c r="A46" s="94"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="90"/>
+      <c r="N46" s="90"/>
+      <c r="O46" s="95"/>
     </row>
     <row r="47" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="101"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="93"/>
-      <c r="F47" s="93"/>
-      <c r="G47" s="93"/>
-      <c r="H47" s="93"/>
-      <c r="I47" s="93"/>
-      <c r="J47" s="93"/>
-      <c r="K47" s="93"/>
-      <c r="L47" s="93"/>
-      <c r="M47" s="93"/>
-      <c r="N47" s="93"/>
-      <c r="O47" s="102"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
+      <c r="M47" s="90"/>
+      <c r="N47" s="90"/>
+      <c r="O47" s="95"/>
     </row>
     <row r="48" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="101"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="93"/>
-      <c r="M48" s="93"/>
-      <c r="N48" s="93"/>
-      <c r="O48" s="102"/>
+      <c r="A48" s="94"/>
+      <c r="B48" s="89"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
+      <c r="M48" s="90"/>
+      <c r="N48" s="90"/>
+      <c r="O48" s="95"/>
     </row>
     <row r="49" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="101"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="92"/>
-      <c r="D49" s="92"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="93"/>
-      <c r="H49" s="93"/>
-      <c r="I49" s="93"/>
-      <c r="J49" s="93"/>
-      <c r="K49" s="93"/>
-      <c r="L49" s="93"/>
-      <c r="M49" s="93"/>
-      <c r="N49" s="93"/>
-      <c r="O49" s="102"/>
+      <c r="A49" s="94"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
+      <c r="M49" s="90"/>
+      <c r="N49" s="90"/>
+      <c r="O49" s="95"/>
     </row>
     <row r="50" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="101"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="92"/>
-      <c r="D50" s="92"/>
-      <c r="E50" s="93"/>
-      <c r="F50" s="93"/>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93"/>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
-      <c r="L50" s="93"/>
-      <c r="M50" s="93"/>
-      <c r="N50" s="93"/>
-      <c r="O50" s="102"/>
+      <c r="A50" s="94"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
+      <c r="M50" s="90"/>
+      <c r="N50" s="90"/>
+      <c r="O50" s="95"/>
     </row>
     <row r="51" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="101"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="92"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="93"/>
-      <c r="F51" s="93"/>
-      <c r="G51" s="93"/>
-      <c r="H51" s="93"/>
-      <c r="I51" s="93"/>
-      <c r="J51" s="93"/>
-      <c r="K51" s="93"/>
-      <c r="L51" s="93"/>
-      <c r="M51" s="93"/>
-      <c r="N51" s="93"/>
-      <c r="O51" s="102"/>
+      <c r="A51" s="94"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
+      <c r="M51" s="90"/>
+      <c r="N51" s="90"/>
+      <c r="O51" s="95"/>
     </row>
     <row r="52" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="101"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="92"/>
-      <c r="D52" s="92"/>
-      <c r="E52" s="93"/>
-      <c r="F52" s="93"/>
-      <c r="G52" s="93"/>
-      <c r="H52" s="93"/>
-      <c r="I52" s="93"/>
-      <c r="J52" s="93"/>
-      <c r="K52" s="93"/>
-      <c r="L52" s="93"/>
-      <c r="M52" s="93"/>
-      <c r="N52" s="93"/>
-      <c r="O52" s="102"/>
+      <c r="A52" s="94"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="90"/>
+      <c r="I52" s="90"/>
+      <c r="J52" s="90"/>
+      <c r="K52" s="90"/>
+      <c r="L52" s="90"/>
+      <c r="M52" s="90"/>
+      <c r="N52" s="90"/>
+      <c r="O52" s="95"/>
     </row>
     <row r="53" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="103"/>
-      <c r="B53" s="104"/>
-      <c r="C53" s="104"/>
-      <c r="D53" s="104"/>
-      <c r="E53" s="104"/>
-      <c r="F53" s="104"/>
-      <c r="G53" s="104"/>
-      <c r="H53" s="104"/>
-      <c r="I53" s="104"/>
-      <c r="J53" s="104"/>
-      <c r="K53" s="104"/>
-      <c r="L53" s="104"/>
-      <c r="M53" s="104"/>
-      <c r="N53" s="104"/>
-      <c r="O53" s="105"/>
+      <c r="A53" s="96"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="97"/>
+      <c r="J53" s="97"/>
+      <c r="K53" s="97"/>
+      <c r="L53" s="97"/>
+      <c r="M53" s="97"/>
+      <c r="N53" s="97"/>
+      <c r="O53" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A36:O36"/>
-    <mergeCell ref="A41:O53"/>
-    <mergeCell ref="A40:O40"/>
-    <mergeCell ref="A39:O39"/>
-    <mergeCell ref="A38:O38"/>
-    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A8:O8"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A2:O2"/>
     <mergeCell ref="A13:O13"/>
     <mergeCell ref="A35:O35"/>
     <mergeCell ref="A34:O34"/>
@@ -14566,18 +14578,12 @@
     <mergeCell ref="A16:O27"/>
     <mergeCell ref="A15:O15"/>
     <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="A9:O9"/>
-    <mergeCell ref="A8:O8"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A5:O5"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="A41:O53"/>
+    <mergeCell ref="A40:O40"/>
+    <mergeCell ref="A39:O39"/>
+    <mergeCell ref="A38:O38"/>
+    <mergeCell ref="A37:O37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -17100,800 +17106,806 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="90"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="104"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="104"/>
     </row>
     <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
     </row>
     <row r="4" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
     </row>
     <row r="6" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
     </row>
     <row r="7" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
     </row>
     <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="89"/>
     </row>
     <row r="9" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="92"/>
-      <c r="O9" s="92"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
     </row>
     <row r="10" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="92"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
     </row>
     <row r="11" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="92"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
     </row>
     <row r="12" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="92"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
     </row>
     <row r="13" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="92"/>
-      <c r="D13" s="92"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="92"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
     </row>
     <row r="14" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
-      <c r="O14" s="92"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
     </row>
     <row r="15" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92"/>
     </row>
     <row r="16" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="101"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="92"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
     </row>
     <row r="17" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="101"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="92"/>
-      <c r="G17" s="92"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="92"/>
-      <c r="N17" s="92"/>
-      <c r="O17" s="92"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
     </row>
     <row r="18" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="101"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="92"/>
-      <c r="M18" s="92"/>
-      <c r="N18" s="92"/>
-      <c r="O18" s="92"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
-      <c r="M19" s="89"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="103"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="103"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
     </row>
     <row r="20" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="89"/>
-      <c r="M20" s="89"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="89"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="103"/>
+      <c r="J20" s="103"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
     </row>
     <row r="21" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="107" t="s">
+      <c r="A21" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="99"/>
-      <c r="M21" s="99"/>
-      <c r="N21" s="99"/>
-      <c r="O21" s="99"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="92"/>
+      <c r="M21" s="92"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="92"/>
     </row>
     <row r="22" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="92"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="92"/>
-      <c r="M22" s="92"/>
-      <c r="N22" s="92"/>
-      <c r="O22" s="92"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="89"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="89"/>
     </row>
     <row r="23" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="92"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="92"/>
-      <c r="O23" s="92"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
     </row>
     <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="92"/>
-      <c r="O24" s="92"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="89"/>
+      <c r="O24" s="89"/>
     </row>
     <row r="25" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
     </row>
     <row r="26" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="92"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="92"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="92"/>
-      <c r="M26" s="92"/>
-      <c r="N26" s="92"/>
-      <c r="O26" s="92"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="89"/>
+      <c r="N26" s="89"/>
+      <c r="O26" s="89"/>
     </row>
     <row r="27" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="92"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="92"/>
-      <c r="M27" s="92"/>
-      <c r="N27" s="92"/>
-      <c r="O27" s="92"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
     </row>
     <row r="28" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="94" t="s">
+      <c r="A28" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="92"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="92"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92"/>
-      <c r="M28" s="92"/>
-      <c r="N28" s="92"/>
-      <c r="O28" s="92"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="89"/>
+      <c r="N28" s="89"/>
+      <c r="O28" s="89"/>
     </row>
     <row r="29" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="91" t="s">
+      <c r="A29" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="92"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="92"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
     </row>
     <row r="30" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="94" t="s">
+      <c r="A30" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="92"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="92"/>
-      <c r="N30" s="92"/>
-      <c r="O30" s="92"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="89"/>
     </row>
     <row r="31" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94" t="s">
+      <c r="A31" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="92"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="89"/>
+      <c r="O31" s="89"/>
     </row>
     <row r="32" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="111"/>
-      <c r="B32" s="104"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="104"/>
-      <c r="F32" s="104"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
-      <c r="L32" s="104"/>
-      <c r="M32" s="104"/>
-      <c r="N32" s="104"/>
-      <c r="O32" s="104"/>
+      <c r="A32" s="107"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+      <c r="N32" s="97"/>
+      <c r="O32" s="97"/>
     </row>
     <row r="33" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
-      <c r="N33" s="99"/>
-      <c r="O33" s="100"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="92"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="92"/>
+      <c r="G33" s="92"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="92"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="92"/>
+      <c r="L33" s="92"/>
+      <c r="M33" s="92"/>
+      <c r="N33" s="92"/>
+      <c r="O33" s="93"/>
     </row>
     <row r="34" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="101"/>
-      <c r="B34" s="92"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="102"/>
+      <c r="A34" s="94"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="95"/>
     </row>
     <row r="35" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="101"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="92"/>
-      <c r="L35" s="92"/>
-      <c r="M35" s="92"/>
-      <c r="N35" s="92"/>
-      <c r="O35" s="102"/>
+      <c r="A35" s="94"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="95"/>
     </row>
     <row r="36" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="101"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
-      <c r="M36" s="92"/>
-      <c r="N36" s="92"/>
-      <c r="O36" s="102"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="95"/>
     </row>
     <row r="37" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="101"/>
-      <c r="B37" s="92"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="92"/>
-      <c r="L37" s="92"/>
-      <c r="M37" s="92"/>
-      <c r="N37" s="92"/>
-      <c r="O37" s="102"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="89"/>
+      <c r="N37" s="89"/>
+      <c r="O37" s="95"/>
     </row>
     <row r="38" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="101"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="92"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="92"/>
-      <c r="I38" s="92"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="92"/>
-      <c r="L38" s="92"/>
-      <c r="M38" s="92"/>
-      <c r="N38" s="92"/>
-      <c r="O38" s="102"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="95"/>
     </row>
     <row r="39" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="101"/>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="92"/>
-      <c r="L39" s="92"/>
-      <c r="M39" s="92"/>
-      <c r="N39" s="92"/>
-      <c r="O39" s="102"/>
+      <c r="A39" s="94"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="89"/>
+      <c r="N39" s="89"/>
+      <c r="O39" s="95"/>
     </row>
     <row r="40" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="101"/>
-      <c r="B40" s="92"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="92"/>
-      <c r="G40" s="92"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="92"/>
-      <c r="L40" s="92"/>
-      <c r="M40" s="92"/>
-      <c r="N40" s="92"/>
-      <c r="O40" s="102"/>
+      <c r="A40" s="94"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="89"/>
+      <c r="N40" s="89"/>
+      <c r="O40" s="95"/>
     </row>
     <row r="41" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="101"/>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="92"/>
-      <c r="G41" s="92"/>
-      <c r="H41" s="92"/>
-      <c r="I41" s="92"/>
-      <c r="J41" s="92"/>
-      <c r="K41" s="92"/>
-      <c r="L41" s="92"/>
-      <c r="M41" s="92"/>
-      <c r="N41" s="92"/>
-      <c r="O41" s="102"/>
+      <c r="A41" s="94"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="89"/>
+      <c r="N41" s="89"/>
+      <c r="O41" s="95"/>
     </row>
     <row r="42" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="101"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="92"/>
-      <c r="H42" s="92"/>
-      <c r="I42" s="92"/>
-      <c r="J42" s="92"/>
-      <c r="K42" s="92"/>
-      <c r="L42" s="92"/>
-      <c r="M42" s="92"/>
-      <c r="N42" s="92"/>
-      <c r="O42" s="102"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="89"/>
+      <c r="J42" s="89"/>
+      <c r="K42" s="89"/>
+      <c r="L42" s="89"/>
+      <c r="M42" s="89"/>
+      <c r="N42" s="89"/>
+      <c r="O42" s="95"/>
     </row>
     <row r="43" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="103"/>
-      <c r="B43" s="104"/>
-      <c r="C43" s="104"/>
-      <c r="D43" s="104"/>
-      <c r="E43" s="104"/>
-      <c r="F43" s="104"/>
-      <c r="G43" s="104"/>
-      <c r="H43" s="104"/>
-      <c r="I43" s="104"/>
-      <c r="J43" s="104"/>
-      <c r="K43" s="104"/>
-      <c r="L43" s="104"/>
-      <c r="M43" s="104"/>
-      <c r="N43" s="104"/>
-      <c r="O43" s="105"/>
+      <c r="A43" s="96"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="97"/>
+      <c r="D43" s="97"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="97"/>
+      <c r="K43" s="97"/>
+      <c r="L43" s="97"/>
+      <c r="M43" s="97"/>
+      <c r="N43" s="97"/>
+      <c r="O43" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="A33:O43"/>
-    <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A31:O31"/>
-    <mergeCell ref="A30:O30"/>
-    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A8:O8"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A5:O5"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A2:O2"/>
     <mergeCell ref="A13:O13"/>
     <mergeCell ref="A27:O27"/>
     <mergeCell ref="A26:O26"/>
@@ -17906,18 +17918,12 @@
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="A15:O18"/>
     <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="A9:O9"/>
-    <mergeCell ref="A8:O8"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A5:O5"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="A33:O43"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="A31:O31"/>
+    <mergeCell ref="A30:O30"/>
+    <mergeCell ref="A29:O29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
@@ -48070,7 +48076,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48571,13 +48577,13 @@
         <v>2976</v>
       </c>
       <c r="C4" t="s">
-        <v>2954</v>
+        <v>4181</v>
       </c>
       <c r="D4" t="s">
         <v>2977</v>
       </c>
       <c r="E4" s="78" t="s">
-        <v>2956</v>
+        <v>4182</v>
       </c>
       <c r="F4" s="78" t="s">
         <v>2957</v>

</xml_diff>